<commit_message>
Implement Modbus/TCP-Slave Api Controller
</commit_message>
<xml_diff>
--- a/io.openems.edge.controller.api.modbus/doc/OpenEMS Modbus-TCP.xlsx
+++ b/io.openems.edge.controller.api.modbus/doc/OpenEMS Modbus-TCP.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stefan.feilmeier\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stefan.feilmeier\fems\develop\io.openems.edge.controller.api.modbus\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{159B5214-B8C0-4D6E-B90C-E7AA8BD3DCCF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A2343A77-31D5-42E8-9F09-71A3E194D30F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{7DF52BB8-339A-45CF-AF24-1A08D3EC1143}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="124">
   <si>
     <t>Address</t>
   </si>
@@ -260,9 +260,6 @@
     <t>e.g. "ess0"</t>
   </si>
   <si>
-    <t>Hash-Code of "SymmetricEss"</t>
-  </si>
-  <si>
     <t>State of Charge</t>
   </si>
   <si>
@@ -293,9 +290,6 @@
     <t>Active Power L3</t>
   </si>
   <si>
-    <t>Hash-Code of "ManagedSymmetricEss"</t>
-  </si>
-  <si>
     <t>…</t>
   </si>
   <si>
@@ -311,9 +305,6 @@
     <t>Set Active Power</t>
   </si>
   <si>
-    <t>RW</t>
-  </si>
-  <si>
     <t>Set Reactive Power</t>
   </si>
   <si>
@@ -390,6 +381,24 @@
   </si>
   <si>
     <t>0xd444b3dc (Hash-Code of "OpenemsComponent")</t>
+  </si>
+  <si>
+    <t>0x1462b (Hash-Code of "Sum")</t>
+  </si>
+  <si>
+    <t>Production: AC Reactive Power</t>
+  </si>
+  <si>
+    <t>Production:Max AC Reactive Power</t>
+  </si>
+  <si>
+    <t>0xbfc142ee (Hash-Code of "SymmetricEss")</t>
+  </si>
+  <si>
+    <t>0xa780a3ed (Hash-Code of "ManagedSymmetricEss")</t>
+  </si>
+  <si>
+    <t>WO</t>
   </si>
 </sst>
 </file>
@@ -465,8 +474,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5D2C3B15-D12B-4604-AC5A-1EC2EF509598}" name="Tabelle1" displayName="Tabelle1" ref="A1:E78" totalsRowShown="0">
-  <autoFilter ref="A1:E78" xr:uid="{C4482380-4FFF-49FE-9B32-93B3B2DF4C66}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5D2C3B15-D12B-4604-AC5A-1EC2EF509598}" name="Tabelle1" displayName="Tabelle1" ref="A1:E82" totalsRowShown="0">
+  <autoFilter ref="A1:E82" xr:uid="{C4482380-4FFF-49FE-9B32-93B3B2DF4C66}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{DD9A594E-1920-4ABF-AE3A-5206941941A7}" name="Address"/>
     <tableColumn id="2" xr3:uid="{B421CB7A-B0D1-4B04-98B4-55971BE572EE}" name="Description"/>
@@ -797,17 +806,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1002D39-991D-4595-BB2E-A9FEB168AA47}">
-  <dimension ref="A1:E78"/>
+  <dimension ref="A1:E82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="34.140625" customWidth="1"/>
     <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -847,7 +856,7 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
@@ -864,7 +873,7 @@
         <v>6</v>
       </c>
       <c r="D4">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
@@ -1043,7 +1052,7 @@
         <v>72</v>
       </c>
       <c r="D15" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E15" t="s">
         <v>7</v>
@@ -1068,7 +1077,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1082,7 +1091,7 @@
         <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E18" t="s">
         <v>7</v>
@@ -1093,7 +1102,7 @@
         <v>221</v>
       </c>
       <c r="B19" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
@@ -1124,7 +1133,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1132,13 +1141,13 @@
         <v>300</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>75</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>36</v>
+        <v>118</v>
       </c>
       <c r="E22" t="s">
         <v>7</v>
@@ -1149,13 +1158,13 @@
         <v>301</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>113</v>
       </c>
       <c r="C23" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" t="s">
-        <v>37</v>
+        <v>6</v>
+      </c>
+      <c r="D23">
+        <v>220</v>
       </c>
       <c r="E23" t="s">
         <v>7</v>
@@ -1163,16 +1172,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C24" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="E24" t="s">
         <v>7</v>
@@ -1180,16 +1189,16 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C25" t="s">
         <v>35</v>
       </c>
       <c r="D25" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="E25" t="s">
         <v>7</v>
@@ -1197,16 +1206,16 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C26" t="s">
         <v>35</v>
       </c>
       <c r="D26" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="E26" t="s">
         <v>7</v>
@@ -1214,16 +1223,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C27" t="s">
         <v>35</v>
       </c>
       <c r="D27" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E27" t="s">
         <v>7</v>
@@ -1231,16 +1240,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C28" t="s">
         <v>35</v>
       </c>
       <c r="D28" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E28" t="s">
         <v>7</v>
@@ -1248,16 +1257,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="B29" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C29" t="s">
         <v>35</v>
       </c>
       <c r="D29" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="E29" t="s">
         <v>7</v>
@@ -1265,16 +1274,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B30" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C30" t="s">
         <v>35</v>
       </c>
       <c r="D30" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E30" t="s">
         <v>7</v>
@@ -1282,16 +1291,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B31" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="C31" t="s">
         <v>35</v>
       </c>
       <c r="D31" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="E31" t="s">
         <v>7</v>
@@ -1299,16 +1308,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B32" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C32" t="s">
         <v>35</v>
       </c>
       <c r="D32" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E32" t="s">
         <v>7</v>
@@ -1316,16 +1325,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C33" t="s">
         <v>35</v>
       </c>
       <c r="D33" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E33" t="s">
         <v>7</v>
@@ -1333,16 +1342,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B34" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="C34" t="s">
         <v>35</v>
       </c>
       <c r="D34" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="E34" t="s">
         <v>7</v>
@@ -1350,16 +1359,16 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B35" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C35" t="s">
         <v>35</v>
       </c>
       <c r="D35" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E35" t="s">
         <v>7</v>
@@ -1367,16 +1376,16 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B36" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C36" t="s">
         <v>35</v>
       </c>
       <c r="D36" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="E36" t="s">
         <v>7</v>
@@ -1384,10 +1393,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B37" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C37" t="s">
         <v>35</v>
@@ -1401,10 +1410,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B38" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C38" t="s">
         <v>35</v>
@@ -1418,10 +1427,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B39" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C39" t="s">
         <v>35</v>
@@ -1435,10 +1444,10 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B40" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C40" t="s">
         <v>35</v>
@@ -1452,16 +1461,16 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="B41" t="s">
-        <v>63</v>
+        <v>119</v>
       </c>
       <c r="C41" t="s">
         <v>35</v>
       </c>
       <c r="D41" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E41" t="s">
         <v>7</v>
@@ -1469,16 +1478,16 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B42" t="s">
-        <v>65</v>
+        <v>120</v>
       </c>
       <c r="C42" t="s">
         <v>35</v>
       </c>
       <c r="D42" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="E42" t="s">
         <v>7</v>
@@ -1486,16 +1495,16 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="B43" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C43" t="s">
         <v>35</v>
       </c>
       <c r="D43" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="E43" t="s">
         <v>7</v>
@@ -1503,42 +1512,50 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
+        <v>339</v>
+      </c>
+      <c r="B44" t="s">
+        <v>62</v>
+      </c>
+      <c r="C44" t="s">
+        <v>35</v>
+      </c>
+      <c r="D44" t="s">
+        <v>46</v>
+      </c>
+      <c r="E44" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>341</v>
+      </c>
+      <c r="B45" t="s">
+        <v>63</v>
+      </c>
+      <c r="C45" t="s">
+        <v>35</v>
+      </c>
+      <c r="D45" t="s">
+        <v>64</v>
+      </c>
+      <c r="E45" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46">
         <v>343</v>
       </c>
-      <c r="B44" t="s">
-        <v>68</v>
-      </c>
-      <c r="C44" t="s">
-        <v>35</v>
-      </c>
-      <c r="D44" t="s">
-        <v>52</v>
-      </c>
-      <c r="E44" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-    </row>
-    <row r="46" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>500</v>
-      </c>
       <c r="B46" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C46" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="D46" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="E46" t="s">
         <v>7</v>
@@ -1546,16 +1563,16 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>516</v>
+        <v>345</v>
       </c>
       <c r="B47" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C47" t="s">
-        <v>6</v>
-      </c>
-      <c r="D47">
-        <v>1000</v>
+        <v>35</v>
+      </c>
+      <c r="D47" t="s">
+        <v>67</v>
       </c>
       <c r="E47" t="s">
         <v>7</v>
@@ -1563,72 +1580,76 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>520</v>
+        <v>347</v>
       </c>
       <c r="B48" t="s">
-        <v>117</v>
+        <v>68</v>
       </c>
       <c r="C48" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="D48" t="s">
-        <v>120</v>
+        <v>52</v>
       </c>
       <c r="E48" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>521</v>
-      </c>
-      <c r="B49" t="s">
-        <v>118</v>
-      </c>
-      <c r="C49" t="s">
-        <v>6</v>
-      </c>
-      <c r="D49">
-        <v>80</v>
-      </c>
-      <c r="E49" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+    </row>
+    <row r="50" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>522</v>
+        <v>500</v>
       </c>
       <c r="B50" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="C50" t="s">
-        <v>6</v>
+        <v>72</v>
       </c>
       <c r="D50" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="E50" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>89</v>
+      <c r="A51">
+        <v>516</v>
+      </c>
+      <c r="B51" t="s">
+        <v>74</v>
+      </c>
+      <c r="C51" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51">
+        <v>1000</v>
+      </c>
+      <c r="E51" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>600</v>
+        <v>520</v>
       </c>
       <c r="B52" t="s">
+        <v>114</v>
+      </c>
+      <c r="C52" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" t="s">
         <v>117</v>
-      </c>
-      <c r="C52" t="s">
-        <v>6</v>
-      </c>
-      <c r="D52" t="s">
-        <v>77</v>
       </c>
       <c r="E52" t="s">
         <v>7</v>
@@ -1636,16 +1657,16 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>601</v>
+        <v>521</v>
       </c>
       <c r="B53" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C53" t="s">
         <v>6</v>
       </c>
       <c r="D53">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="E53" t="s">
         <v>7</v>
@@ -1653,55 +1674,55 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>602</v>
+        <v>522</v>
       </c>
       <c r="B54" t="s">
-        <v>78</v>
+        <v>27</v>
       </c>
       <c r="C54" t="s">
         <v>6</v>
       </c>
       <c r="D54" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E54" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>603</v>
-      </c>
-      <c r="B55" t="s">
-        <v>79</v>
-      </c>
-      <c r="C55" t="s">
-        <v>6</v>
-      </c>
-      <c r="D55" t="s">
-        <v>83</v>
-      </c>
-      <c r="E55" t="s">
-        <v>7</v>
+      <c r="A55" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>89</v>
+      <c r="A56">
+        <v>600</v>
+      </c>
+      <c r="B56" t="s">
+        <v>114</v>
+      </c>
+      <c r="C56" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56" t="s">
+        <v>121</v>
+      </c>
+      <c r="E56" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>700</v>
+        <v>601</v>
       </c>
       <c r="B57" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C57" t="s">
         <v>6</v>
       </c>
-      <c r="D57" t="s">
-        <v>84</v>
+      <c r="D57">
+        <v>100</v>
       </c>
       <c r="E57" t="s">
         <v>7</v>
@@ -1709,16 +1730,16 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>701</v>
+        <v>602</v>
       </c>
       <c r="B58" t="s">
-        <v>118</v>
+        <v>77</v>
       </c>
       <c r="C58" t="s">
         <v>6</v>
       </c>
-      <c r="D58">
-        <v>100</v>
+      <c r="D58" t="s">
+        <v>36</v>
       </c>
       <c r="E58" t="s">
         <v>7</v>
@@ -1726,72 +1747,72 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>702</v>
+        <v>603</v>
       </c>
       <c r="B59" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C59" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="D59" t="s">
-        <v>37</v>
+        <v>82</v>
       </c>
       <c r="E59" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>704</v>
-      </c>
-      <c r="B60" t="s">
-        <v>86</v>
-      </c>
-      <c r="C60" t="s">
-        <v>35</v>
-      </c>
-      <c r="D60" t="s">
-        <v>37</v>
-      </c>
-      <c r="E60" t="s">
-        <v>7</v>
+      <c r="A60" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>706</v>
+        <v>700</v>
       </c>
       <c r="B61" t="s">
-        <v>87</v>
+        <v>114</v>
       </c>
       <c r="C61" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="D61" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="E61" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>89</v>
+      <c r="A62">
+        <v>701</v>
+      </c>
+      <c r="B62" t="s">
+        <v>115</v>
+      </c>
+      <c r="C62" t="s">
+        <v>6</v>
+      </c>
+      <c r="D62">
+        <v>100</v>
+      </c>
+      <c r="E62" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>800</v>
+        <v>702</v>
       </c>
       <c r="B63" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="C63" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="D63" t="s">
-        <v>88</v>
+        <v>37</v>
       </c>
       <c r="E63" t="s">
         <v>7</v>
@@ -1799,16 +1820,16 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>801</v>
+        <v>704</v>
       </c>
       <c r="B64" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
       <c r="C64" t="s">
-        <v>6</v>
-      </c>
-      <c r="D64">
-        <v>100</v>
+        <v>35</v>
+      </c>
+      <c r="D64" t="s">
+        <v>37</v>
       </c>
       <c r="E64" t="s">
         <v>7</v>
@@ -1816,203 +1837,259 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>802</v>
+        <v>706</v>
       </c>
       <c r="B65" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C65" t="s">
         <v>35</v>
       </c>
       <c r="D65" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="E65" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>804</v>
-      </c>
-      <c r="B66" t="s">
-        <v>91</v>
-      </c>
-      <c r="C66" t="s">
-        <v>35</v>
-      </c>
-      <c r="D66" t="s">
-        <v>46</v>
-      </c>
-      <c r="E66" t="s">
-        <v>7</v>
+      <c r="A66" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>806</v>
+        <v>800</v>
       </c>
       <c r="B67" t="s">
-        <v>93</v>
+        <v>114</v>
       </c>
       <c r="C67" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="D67" t="s">
-        <v>37</v>
+        <v>122</v>
       </c>
       <c r="E67" t="s">
-        <v>94</v>
+        <v>7</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>808</v>
+        <v>801</v>
       </c>
       <c r="B68" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="C68" t="s">
-        <v>35</v>
-      </c>
-      <c r="D68" t="s">
-        <v>38</v>
+        <v>6</v>
+      </c>
+      <c r="D68">
+        <v>100</v>
       </c>
       <c r="E68" t="s">
-        <v>94</v>
+        <v>7</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>810</v>
+        <v>802</v>
       </c>
       <c r="B69" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C69" t="s">
         <v>35</v>
       </c>
       <c r="D69" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="E69" t="s">
-        <v>94</v>
+        <v>7</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>812</v>
+        <v>804</v>
       </c>
       <c r="B70" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C70" t="s">
         <v>35</v>
       </c>
       <c r="D70" t="s">
+        <v>46</v>
+      </c>
+      <c r="E70" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>806</v>
+      </c>
+      <c r="B71" t="s">
+        <v>91</v>
+      </c>
+      <c r="C71" t="s">
+        <v>35</v>
+      </c>
+      <c r="D71" t="s">
         <v>37</v>
       </c>
-      <c r="E70" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>89</v>
+      <c r="E71" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>900</v>
+        <v>808</v>
       </c>
       <c r="B72" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="C72" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="D72" t="s">
-        <v>92</v>
+        <v>38</v>
       </c>
       <c r="E72" t="s">
-        <v>7</v>
+        <v>123</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>901</v>
+        <v>810</v>
       </c>
       <c r="B73" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="C73" t="s">
-        <v>6</v>
-      </c>
-      <c r="D73">
-        <v>100</v>
+        <v>35</v>
+      </c>
+      <c r="D73" t="s">
+        <v>37</v>
       </c>
       <c r="E73" t="s">
-        <v>7</v>
+        <v>123</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>89</v>
+      <c r="A74">
+        <v>812</v>
+      </c>
+      <c r="B74" t="s">
+        <v>95</v>
+      </c>
+      <c r="C74" t="s">
+        <v>35</v>
+      </c>
+      <c r="D74" t="s">
+        <v>37</v>
+      </c>
+      <c r="E74" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>1000</v>
-      </c>
-      <c r="B75" t="s">
-        <v>117</v>
-      </c>
-      <c r="C75" t="s">
-        <v>6</v>
-      </c>
-      <c r="D75" t="s">
-        <v>96</v>
-      </c>
-      <c r="E75" t="s">
-        <v>7</v>
+      <c r="A75" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
+        <v>900</v>
+      </c>
+      <c r="B76" t="s">
+        <v>114</v>
+      </c>
+      <c r="C76" t="s">
+        <v>6</v>
+      </c>
+      <c r="D76" t="s">
+        <v>90</v>
+      </c>
+      <c r="E76" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>901</v>
+      </c>
+      <c r="B77" t="s">
+        <v>115</v>
+      </c>
+      <c r="C77" t="s">
+        <v>6</v>
+      </c>
+      <c r="D77">
+        <v>100</v>
+      </c>
+      <c r="E77" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>1000</v>
+      </c>
+      <c r="B79" t="s">
+        <v>114</v>
+      </c>
+      <c r="C79" t="s">
+        <v>6</v>
+      </c>
+      <c r="D79" t="s">
+        <v>93</v>
+      </c>
+      <c r="E79" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80">
         <v>1001</v>
       </c>
-      <c r="B76" t="s">
-        <v>118</v>
-      </c>
-      <c r="C76" t="s">
-        <v>6</v>
-      </c>
-      <c r="D76">
+      <c r="B80" t="s">
+        <v>115</v>
+      </c>
+      <c r="C80" t="s">
+        <v>6</v>
+      </c>
+      <c r="D80">
         <v>300</v>
       </c>
-      <c r="E76" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78">
+      <c r="E80" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82">
         <v>1300</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B82" t="s">
         <v>70</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C82" t="s">
         <v>71</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D82" t="s">
         <v>73</v>
       </c>
-      <c r="E78" t="s">
+      <c r="E82" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2085,7 +2162,7 @@
     </row>
     <row r="7" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" s="1"/>
     </row>
@@ -2094,7 +2171,7 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2102,7 +2179,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -2110,7 +2187,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2137,66 +2214,66 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" t="s">
         <v>110</v>
-      </c>
-      <c r="B7" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B8" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>